<commit_message>
Model & Graphics updation
</commit_message>
<xml_diff>
--- a/DeepaliNarkhede/Training01/Training01/ProgressReport/Progress Report_PB_3july20.xlsx
+++ b/DeepaliNarkhede/Training01/Training01/ProgressReport/Progress Report_PB_3july20.xlsx
@@ -260,17 +260,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,11 +294,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -364,41 +364,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -427,6 +392,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -442,34 +414,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2126,40 +2070,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="9"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -2203,7 +2147,7 @@
       <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2277,12 +2221,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2385,7 +2329,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="16" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="14" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2426,13 +2370,13 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="16" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q2" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="14" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2444,13 +2388,13 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="16" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="14" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2464,15 +2408,15 @@
       <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="16" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="14" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -2482,15 +2426,15 @@
       <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="17" t="s">
+      <c r="Q5" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="14" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2500,13 +2444,13 @@
       <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="18"/>
+      <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="1:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -2516,9 +2460,9 @@
       <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="13"/>
-    </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" s="14" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2532,9 +2476,9 @@
       <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" s="14" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2549,7 +2493,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="14" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2564,7 +2508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="16" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="14" customFormat="1" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2580,60 +2524,60 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2833,7 +2777,7 @@
       <c r="E3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2849,7 +2793,7 @@
       <c r="E4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2865,7 +2809,7 @@
       <c r="E5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="20" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2881,7 +2825,7 @@
       <c r="E6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="19" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>